<commit_message>
updated marketing user pages
</commit_message>
<xml_diff>
--- a/data/CustomerPortalTestData.xlsx
+++ b/data/CustomerPortalTestData.xlsx
@@ -128,7 +128,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -194,12 +194,6 @@
       <name val="Consolas"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -306,7 +300,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,7 +436,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.6"/>
   </cols>
@@ -584,7 +578,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changes in test cases and data
</commit_message>
<xml_diff>
--- a/data/CustomerPortalTestData.xlsx
+++ b/data/CustomerPortalTestData.xlsx
@@ -5,13 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MarketingUser" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ManageUser" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="ManageMarketingUser" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="MarketingLogin" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="RevenueSummary" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="RevenueSummaryDate" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="RevenueSummaryPublication" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="RevenueSummarySalesOffice" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Agency" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="BranchData" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -119,6 +126,234 @@
   <si>
     <t xml:space="preserve">Marketing Executive</t>
   </si>
+  <si>
+    <t xml:space="preserve">8021vac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARGHESE CHANDY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SalesOffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jun 2021 - Dec 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCHIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANORAMA DAILY DISPLAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Target(INR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Actual(INR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variance(INR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Achievement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY-Revenue Actual(INR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">164000000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41054396.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122945603.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208878664.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-80.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANORAMA WEEKLY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3200000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">141950.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3058050.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475325.74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-70.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THE WEEK - REGULAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">74000000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">325550.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73674449.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387281.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANORAMA DAILY DISPLAY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">149000000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35429848.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113570151.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129461576.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-72.63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2400000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">495500.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-100.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102000000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83520.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101916479.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450000.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-81.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agency Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postal Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0006021402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCESS COMMUNICATIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRICHUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bijuaccess@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9847189952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">680001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRISSUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0006019277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0006019487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &amp; A ADVERTISING &amp; MARKETING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerala</t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -195,6 +430,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -251,7 +492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,6 +543,18 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -425,6 +678,143 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="bijuaccess@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -436,7 +826,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.6"/>
   </cols>
@@ -577,7 +967,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -623,4 +1013,545 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="18.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="18.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="18.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>